<commit_message>
Cambios ultimos del dia, importantes
hoy
</commit_message>
<xml_diff>
--- a/maiaa.xlsx
+++ b/maiaa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Autores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073896A4-635F-4585-BCDD-E827F33BE6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC4873-EA89-498D-B13B-B42FB74E56D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Brito Borges</t>
   </si>
   <si>
-    <t>ejemlo@.com</t>
-  </si>
-  <si>
-    <t>facebook.com.mx</t>
-  </si>
-  <si>
     <t>Encargado del desarrollo primordial de la API de la plataforma.</t>
   </si>
   <si>
@@ -75,31 +69,43 @@
     <t>dsssssss</t>
   </si>
   <si>
-    <t>dssssssssss</t>
-  </si>
-  <si>
-    <t>dssssss</t>
-  </si>
-  <si>
-    <t>sddddddd</t>
-  </si>
-  <si>
-    <t>sddddddddddddddddd</t>
-  </si>
-  <si>
-    <t>jjj</t>
-  </si>
-  <si>
-    <t>hhhhh</t>
-  </si>
-  <si>
-    <t>iiii</t>
-  </si>
-  <si>
     <t>junior</t>
   </si>
   <si>
     <t>senior</t>
+  </si>
+  <si>
+    <t>https://mx.linkedin.com/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/intl/es-419/gmail/about/</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>Orizco del Castillo</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Gongora Bojorquez</t>
+  </si>
+  <si>
+    <t>Uicab</t>
+  </si>
+  <si>
+    <t>Jose Luis</t>
+  </si>
+  <si>
+    <t>Uicab can</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Caamal Castañeda</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +167,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -442,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,7 +464,7 @@
     <col min="7" max="7" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -488,88 +498,88 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -580,19 +590,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -603,19 +613,19 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -626,19 +636,19 @@
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -649,102 +659,120 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F17" s="3"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D759A46F-8933-4FCC-A3AD-5EBF9988A509}"/>
-    <hyperlink ref="D3:D9" r:id="rId2" display="ejemlo@.com" xr:uid="{AF80A2B2-11E5-45D2-A5F5-377A3DE2EC55}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{5FCC2FE3-11AF-43E7-8FB5-C4E6F45C2F38}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{1DADAD36-5269-4C59-B54C-E630F7C0FB33}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{65677745-9717-4CE4-90C8-2E64DC4409E0}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{8B486DED-10FE-4EF5-9924-A54E9FCB9507}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{05D08F20-132A-4A68-B233-F2BA562366EA}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{5C874E48-C8D0-4336-94C2-76D7057A3C8C}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{BAF4EDE5-DB7E-4259-8A42-D3C65BEE8589}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{BD996624-F8E1-4E6D-9DD8-0AF5C1132363}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{4558B58C-B663-463C-970B-46133A3D172F}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{7B71DC2E-D6DB-49C3-8ABF-0E8BB15C37BE}"/>
+    <hyperlink ref="D3" r:id="rId11" xr:uid="{6A2FBEFA-6D24-41C7-B56F-D3D5956D9DA2}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{D3BC2717-9EEA-4374-965B-87E1D662A5B9}"/>
+    <hyperlink ref="D11" r:id="rId13" xr:uid="{09E322AB-847A-4B95-B7B6-FE1B3003E613}"/>
+    <hyperlink ref="D12" r:id="rId14" xr:uid="{6AE5B2D3-E276-40F3-B9CD-AD1C01C8694B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>